<commit_message>
KD model update, scrapper update
Signed-off-by: Léa Chateauneuf <lea.chateauneuf@kapcode.fr>
</commit_message>
<xml_diff>
--- a/KD model/NLP4StatRef-CrossMapping_20210605.xlsx
+++ b/KD model/NLP4StatRef-CrossMapping_20210605.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Pro\LuapLab\Prestations\Union Européenne\Eurostat\KnowledgeDatabase\Mappings\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{612A46EB-5030-4D9D-914D-A1DB1615E6AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{478A8EE0-E08D-4D82-AB9E-AEBD78509AF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="19392" windowHeight="10536" firstSheet="1" activeTab="1" xr2:uid="{548EE817-9B61-4AD1-B105-CBD7F5BE79FF}"/>
   </bookViews>
@@ -20,7 +20,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'KD-LinkTarget'!$A$1:$N$51</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1469,11 +1469,11 @@
   <dimension ref="A1:N51"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="7896" ySplit="480" topLeftCell="I37" activePane="bottomRight"/>
+      <pane xSplit="7896" ySplit="480" topLeftCell="I34" activePane="bottomRight"/>
       <selection activeCell="B1" sqref="B1:B1048576"/>
       <selection pane="topRight" activeCell="K2" sqref="K2"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="L41" sqref="L41:N41"/>
+      <selection pane="bottomRight" activeCell="J47" sqref="J47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.7" x14ac:dyDescent="0.65"/>

</xml_diff>